<commit_message>
worked on fronend integration
</commit_message>
<xml_diff>
--- a/public/import-templates/products-template.xlsx
+++ b/public/import-templates/products-template.xlsx
@@ -61,117 +61,167 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Product SKU</t>
+          <t>Product Name</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Product Name</t>
+          <t>SEO Slug</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Product Type</t>
+          <t>Status</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Status</t>
+          <t>Short Description</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Price</t>
+          <t>Description</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Sale Price</t>
+          <t>Brand Slugs (comma separated)</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Brand Slugs (comma separated)</t>
+          <t>Category Slugs (comma separated)</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Category Slugs (comma separated)</t>
+          <t>Tag List</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Tag List</t>
+          <t>Featured</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Description</t>
+          <t>Requires Shipping (0 or 1)</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Short Description</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+          <t>Free Shipping (0 or 1)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>GST Type (0 or 1)</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>GST Percentage</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Meta Title</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Meta Description</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Meta Keywords</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>SKU-001</t>
+          <t>Sample T-Shirt</t>
         </is>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>Sample Product</t>
+          <t>sample-t-shirt</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>variable</t>
+          <t>published</t>
         </is>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>hidden</t>
+          <t>A comfortable cotton t-shirt for everyday wear</t>
         </is>
       </c>
       <c r="E2" s="0" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>&lt;p&gt;This is a high-quality cotton t-shirt that offers comfort and style. Perfect for casual wear.&lt;/p&gt;</t>
         </is>
       </c>
       <c r="F2" s="0" t="inlineStr">
         <is>
-          <t>90.00</t>
+          <t>other, brand-name</t>
         </is>
       </c>
       <c r="G2" s="0" t="inlineStr">
         <is>
-          <t>other</t>
+          <t>clothing, mens-clothing</t>
         </is>
       </c>
       <c r="H2" s="0" t="inlineStr">
         <is>
-          <t>home-appliances|kitchen-appliances</t>
+          <t>casual, cotton, comfortable</t>
         </is>
       </c>
       <c r="I2" s="0" t="inlineStr">
         <is>
-          <t>tag1, tag2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="J2" s="0" t="inlineStr">
         <is>
-          <t>&lt;p&gt;Main content here&lt;/p&gt;</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K2" s="0" t="inlineStr">
         <is>
-          <t>Quick summary</t>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L2" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M2" s="0" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="N2" s="0" t="inlineStr">
+        <is>
+          <t>Sample T-Shirt - Comfortable Cotton</t>
+        </is>
+      </c>
+      <c r="O2" s="0" t="inlineStr">
+        <is>
+          <t>Buy our comfortable cotton t-shirt. Perfect for everyday wear.</t>
+        </is>
+      </c>
+      <c r="P2" s="0" t="inlineStr">
+        <is>
+          <t>t-shirt, cotton, casual, clothing</t>
         </is>
       </c>
     </row>
@@ -182,147 +232,152 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:21">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Product SKU</t>
+          <t>Product Name</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Product Slug</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Variant SKU</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Variant Name</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Sale Price</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Cost Price</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Stock Quantity</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Manage Stock (0 or 1)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Stock Status</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Is Active (0 or 1)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Attributes JSON</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Price</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Sale Price</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Cost Price</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Stock Quantity</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Manage Stock (0 or 1)</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Stock Status</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Is Active (0 or 1)</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Weight</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Length</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Width</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Height</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Diameter</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Discount Type</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Discount Value</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Discount Active</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Measurements JSON</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Weight</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Length</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Width</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Height</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Diameter</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>SKU-001</t>
+          <t>Sample T-Shirt</t>
         </is>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>SKU-001-V1</t>
+          <t>sample-t-shirt</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>Variant Option 1</t>
+          <t>TSHIRT-RED-M</t>
         </is>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>{"color":"Black","storage":"128GB"}</t>
+          <t>Red - Medium</t>
         </is>
       </c>
       <c r="E2" s="0" t="inlineStr">
         <is>
-          <t>100.00</t>
+          <t>29.99</t>
         </is>
       </c>
       <c r="F2" s="0" t="inlineStr">
         <is>
-          <t>90.00</t>
+          <t>24.99</t>
         </is>
       </c>
       <c r="G2" s="0" t="inlineStr">
         <is>
-          <t>80.00</t>
+          <t>15.00</t>
         </is>
       </c>
       <c r="H2" s="0" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>50</t>
         </is>
       </c>
       <c r="I2" s="0" t="inlineStr">
@@ -342,20 +397,159 @@
       </c>
       <c r="L2" s="0" t="inlineStr">
         <is>
+          <t>{"color":"red","size":"M"}</t>
+        </is>
+      </c>
+      <c r="M2" s="0" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="R2" s="0" t="inlineStr">
+        <is>
           <t>percentage</t>
         </is>
       </c>
-      <c r="M2" s="0" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="N2" s="0" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="O2" s="0" t="inlineStr">
+      <c r="S2" s="0" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="T2" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U2" s="0" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>Sample T-Shirt</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>TSHIRT-RED-L</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>Red - Large</t>
+        </is>
+      </c>
+      <c r="E3" s="0" t="inlineStr">
+        <is>
+          <t>29.99</t>
+        </is>
+      </c>
+      <c r="F3" s="0" t="inlineStr">
+        <is>
+          <t>24.99</t>
+        </is>
+      </c>
+      <c r="G3" s="0" t="inlineStr">
+        <is>
+          <t>15.00</t>
+        </is>
+      </c>
+      <c r="H3" s="0" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="I3" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J3" s="0" t="inlineStr">
+        <is>
+          <t>in_stock</t>
+        </is>
+      </c>
+      <c r="K3" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L3" s="0" t="inlineStr">
+        <is>
+          <t>{"color":"red","size":"L"}</t>
+        </is>
+      </c>
+      <c r="M3" s="0" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="U3" s="0" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>Sample T-Shirt</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>TSHIRT-BLUE-M</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>Blue - Medium</t>
+        </is>
+      </c>
+      <c r="E4" s="0" t="inlineStr">
+        <is>
+          <t>29.99</t>
+        </is>
+      </c>
+      <c r="G4" s="0" t="inlineStr">
+        <is>
+          <t>15.00</t>
+        </is>
+      </c>
+      <c r="H4" s="0" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="I4" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J4" s="0" t="inlineStr">
+        <is>
+          <t>in_stock</t>
+        </is>
+      </c>
+      <c r="K4" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L4" s="0" t="inlineStr">
+        <is>
+          <t>{"color":"blue","size":"M"}</t>
+        </is>
+      </c>
+      <c r="M4" s="0" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="U4" s="0" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -368,84 +562,121 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Product SKU</t>
+          <t>Product Name</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Product Slug</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Image Path or URL</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Is Primary (0 or 1)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Sort Order</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Alt Text</t>
         </is>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>SKU-001</t>
+          <t>Sample T-Shirt</t>
         </is>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>products/sample-primary.jpg</t>
+          <t>sample-t-shirt</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>products/sample-t-shirt-front.jpg</t>
         </is>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E2" s="0" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E2" s="0" t="inlineStr">
-        <is>
-          <t>Front profile</t>
-        </is>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="0" t="inlineStr">
+        <is>
+          <t>Sample T-Shirt Front View</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>SKU-001</t>
-        </is>
-      </c>
-      <c r="B3" s="0" t="inlineStr">
-        <is>
-          <t>products/sample-secondary.jpg</t>
+          <t>Sample T-Shirt</t>
         </is>
       </c>
       <c r="C3" s="0" t="inlineStr">
         <is>
+          <t>products/sample-t-shirt-back.jpg</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="D3" s="0" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="E3" s="0" t="inlineStr">
         <is>
-          <t>Lifestyle photo</t>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F3" s="0" t="inlineStr">
+        <is>
+          <t>Sample T-Shirt Back View</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>Sample T-Shirt</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>products/sample-t-shirt-side.jpg</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E4" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F4" s="0" t="inlineStr">
+        <is>
+          <t>Sample T-Shirt Side View</t>
         </is>
       </c>
     </row>

</xml_diff>